<commit_message>
Update--phrase deck now has stories
</commit_message>
<xml_diff>
--- a/Steno practice log.xlsx
+++ b/Steno practice log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="593">
   <si>
     <t>Date</t>
   </si>
@@ -3838,6 +3838,21 @@
   </si>
   <si>
     <t>Focused on adding in stories for phrase card deck today. I added in about 169 stories today and have now added in a total of 449 (through phrase #814). I'm guessing that I have about 160 more stories to add in.</t>
+  </si>
+  <si>
+    <r>
+      <t>Finished adding stories to phrase deck! There are currently 629 stories in the phrase deck. Wow, that only took 3 days!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I also uploaded this new phrase deck to Anki. I made 5 changes to the outlines in my single-word deck today.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5431,11 +5446,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="527515896"/>
-        <c:axId val="527514328"/>
+        <c:axId val="341720640"/>
+        <c:axId val="341716328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="527515896"/>
+        <c:axId val="341720640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5477,7 +5492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527514328"/>
+        <c:crossAx val="341716328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5485,7 +5500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527514328"/>
+        <c:axId val="341716328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5536,7 +5551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527515896"/>
+        <c:crossAx val="341720640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6106,11 +6121,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="527521384"/>
-        <c:axId val="527515112"/>
+        <c:axId val="341718680"/>
+        <c:axId val="341721816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="527521384"/>
+        <c:axId val="341718680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6152,7 +6167,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527515112"/>
+        <c:crossAx val="341721816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6160,7 +6175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527515112"/>
+        <c:axId val="341721816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6211,7 +6226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527521384"/>
+        <c:crossAx val="341718680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6452,11 +6467,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="527515504"/>
-        <c:axId val="527517464"/>
+        <c:axId val="341719072"/>
+        <c:axId val="341718288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="527515504"/>
+        <c:axId val="341719072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6498,7 +6513,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527517464"/>
+        <c:crossAx val="341718288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6506,7 +6521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527517464"/>
+        <c:axId val="341718288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -6559,7 +6574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527515504"/>
+        <c:crossAx val="341719072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6828,11 +6843,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="527519424"/>
-        <c:axId val="527516680"/>
+        <c:axId val="341715936"/>
+        <c:axId val="341717112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="527519424"/>
+        <c:axId val="341715936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6874,7 +6889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527516680"/>
+        <c:crossAx val="341717112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6882,7 +6897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527516680"/>
+        <c:axId val="341717112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6934,7 +6949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527519424"/>
+        <c:crossAx val="341715936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9664,11 +9679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF603"/>
+  <dimension ref="A1:AF604"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="17" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B606" sqref="B606"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="17" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P605" sqref="P605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9879,7 +9894,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="60">
         <f>SUM(B18:B1000036)</f>
-        <v>1623.5799999999974</v>
+        <v>1630.9799999999975</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -23785,6 +23800,29 @@
       </c>
       <c r="V603" s="16" t="s">
         <v>591</v>
+      </c>
+    </row>
+    <row r="604" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A604" s="4">
+        <v>43878</v>
+      </c>
+      <c r="B604" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="M604" s="10">
+        <v>0</v>
+      </c>
+      <c r="N604" s="46">
+        <v>0</v>
+      </c>
+      <c r="T604" s="10">
+        <v>1293</v>
+      </c>
+      <c r="U604" s="61">
+        <v>1079</v>
+      </c>
+      <c r="V604" s="2" t="s">
+        <v>592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update and happy Leap Day
</commit_message>
<xml_diff>
--- a/Steno practice log.xlsx
+++ b/Steno practice log.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="599">
   <si>
     <t>Date</t>
   </si>
@@ -3868,6 +3868,9 @@
   </si>
   <si>
     <t>Made one outline change today. (Note: there are now 1080 cards in the phrase deck.)</t>
+  </si>
+  <si>
+    <t>Lol at column L. Haven't made any changes to single-word deck outlines in a couple of days, I think</t>
   </si>
 </sst>
 </file>
@@ -4159,13 +4162,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>%</a:t>
+              <a:t>% of single-word deck card reviews that were correct</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Single-word deck card reviews correct</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4231,10 +4229,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$73:$F$601</c:f>
+              <c:f>Sheet1!$F$73:$F$613</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="529"/>
+                <c:ptCount val="541"/>
                 <c:pt idx="0">
                   <c:v>62.8</c:v>
                 </c:pt>
@@ -5446,6 +5444,36 @@
                 </c:pt>
                 <c:pt idx="528">
                   <c:v>82.3</c:v>
+                </c:pt>
+                <c:pt idx="529">
+                  <c:v>84.9</c:v>
+                </c:pt>
+                <c:pt idx="532">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="533">
+                  <c:v>77.3</c:v>
+                </c:pt>
+                <c:pt idx="534">
+                  <c:v>80.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="535">
+                  <c:v>83.4</c:v>
+                </c:pt>
+                <c:pt idx="536">
+                  <c:v>88.6</c:v>
+                </c:pt>
+                <c:pt idx="537">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="538">
+                  <c:v>85.9</c:v>
+                </c:pt>
+                <c:pt idx="539">
+                  <c:v>81.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="540">
+                  <c:v>89.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5461,11 +5489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="426180144"/>
-        <c:axId val="426178184"/>
+        <c:axId val="136418000"/>
+        <c:axId val="136417608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426180144"/>
+        <c:axId val="136418000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5507,7 +5535,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426178184"/>
+        <c:crossAx val="136417608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5515,7 +5543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426178184"/>
+        <c:axId val="136417608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5566,7 +5594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426180144"/>
+        <c:crossAx val="136418000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5650,7 +5678,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Non-mature outlines left in</a:t>
+              <a:t>Non-mature cards left in</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -5660,6 +5688,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5722,10 +5751,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$423:$T$601</c:f>
+              <c:f>Sheet1!$T$423:$T$613</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="179"/>
+                <c:ptCount val="191"/>
                 <c:pt idx="0">
                   <c:v>285</c:v>
                 </c:pt>
@@ -6121,6 +6150,42 @@
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>1362</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1287</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1288</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1293</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1168</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1086</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>893</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>803</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6136,11 +6201,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="426183672"/>
-        <c:axId val="426181712"/>
+        <c:axId val="432416416"/>
+        <c:axId val="432422688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426183672"/>
+        <c:axId val="432416416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6182,7 +6247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426181712"/>
+        <c:crossAx val="432422688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6190,7 +6255,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426181712"/>
+        <c:axId val="432422688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6241,7 +6306,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426183672"/>
+        <c:crossAx val="432416416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6383,10 +6448,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$576:$M$612</c:f>
+              <c:f>Sheet1!$M$576:$M$613</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6490,6 +6555,9 @@
                   <c:v>4201</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>4201</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>4201</c:v>
                 </c:pt>
               </c:numCache>
@@ -6506,11 +6574,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="426182888"/>
-        <c:axId val="426180928"/>
+        <c:axId val="432421512"/>
+        <c:axId val="432418376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426182888"/>
+        <c:axId val="432421512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6552,7 +6620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426180928"/>
+        <c:crossAx val="432418376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6560,7 +6628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426180928"/>
+        <c:axId val="432418376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -6613,7 +6681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426182888"/>
+        <c:crossAx val="432421512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6663,411 +6731,6 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number of</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> non-mature cards in single-word deck</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$T$577:$T$612</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>4201</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4201</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4201</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4201</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4197</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4177</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3957</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3502</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3457</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3352</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3238</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3201</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3035</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2895</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2875</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2736</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2579</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2331</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2193</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1956</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1818</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1719</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1501</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1362</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1287</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1288</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1293</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1168</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1086</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>931</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>893</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>850</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>803</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>756</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>731</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$U$577:$U$597</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="426182104"/>
-        <c:axId val="426181320"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="426182104"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="426181320"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="426181320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="426182104"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7165,10 +6828,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$608:$N$612</c:f>
+              <c:f>Sheet1!$N$608:$N$613</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -7180,6 +6843,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7195,11 +6861,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="426177792"/>
-        <c:axId val="426183280"/>
+        <c:axId val="432422296"/>
+        <c:axId val="432416024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426177792"/>
+        <c:axId val="432422296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7241,7 +6907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426183280"/>
+        <c:crossAx val="432416024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7249,7 +6915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426183280"/>
+        <c:axId val="432416024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7300,7 +6966,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426177792"/>
+        <c:crossAx val="432422296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7349,7 +7015,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7447,10 +7113,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$608:$U$612</c:f>
+              <c:f>Sheet1!$U$608:$U$613</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1080</c:v>
                 </c:pt>
@@ -7465,6 +7131,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7480,11 +7149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="426184064"/>
-        <c:axId val="426179752"/>
+        <c:axId val="432421904"/>
+        <c:axId val="432419552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="426184064"/>
+        <c:axId val="432421904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7526,7 +7195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426179752"/>
+        <c:crossAx val="432419552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7534,7 +7203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426179752"/>
+        <c:axId val="432419552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7585,7 +7254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426184064"/>
+        <c:crossAx val="432421904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7795,46 +7464,6 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10454,536 +10083,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>543069</xdr:colOff>
-      <xdr:row>493</xdr:row>
-      <xdr:rowOff>92172</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>244896</xdr:colOff>
+      <xdr:row>652</xdr:row>
+      <xdr:rowOff>9345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>498464</xdr:colOff>
-      <xdr:row>527</xdr:row>
-      <xdr:rowOff>130272</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>2577400</xdr:colOff>
+      <xdr:row>686</xdr:row>
+      <xdr:rowOff>47445</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11004,16 +10117,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>23811</xdr:colOff>
-      <xdr:row>529</xdr:row>
-      <xdr:rowOff>55563</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520767</xdr:colOff>
+      <xdr:row>619</xdr:row>
+      <xdr:rowOff>121823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>539</xdr:row>
-      <xdr:rowOff>100543</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1316934</xdr:colOff>
+      <xdr:row>633</xdr:row>
+      <xdr:rowOff>8282</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11057,36 +10170,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>244734</xdr:colOff>
-      <xdr:row>621</xdr:row>
-      <xdr:rowOff>62226</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>927652</xdr:colOff>
-      <xdr:row>633</xdr:row>
-      <xdr:rowOff>173935</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11185,7 +10268,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11215,7 +10298,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11487,11 +10570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF612"/>
+  <dimension ref="A1:AF613"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="17" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V621" sqref="V621"/>
+      <pane ySplit="17" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V614" sqref="V614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11702,7 +10785,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="60">
         <f>SUM(B18:B1000055)</f>
-        <v>1643.8799999999976</v>
+        <v>1648.1799999999976</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -11728,7 +10811,7 @@
       </c>
       <c r="D16" s="59">
         <f>SUM(C45:D1000054)</f>
-        <v>119105</v>
+        <v>120277</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -25899,6 +24982,47 @@
       </c>
       <c r="U612" s="61">
         <v>860</v>
+      </c>
+    </row>
+    <row r="613" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A613" s="4">
+        <v>43889</v>
+      </c>
+      <c r="B613" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="C613" s="10">
+        <v>185</v>
+      </c>
+      <c r="D613" s="46">
+        <v>987</v>
+      </c>
+      <c r="F613" s="10">
+        <v>89.2</v>
+      </c>
+      <c r="L613" s="47">
+        <v>35.9</v>
+      </c>
+      <c r="M613" s="10">
+        <v>4201</v>
+      </c>
+      <c r="N613" s="46">
+        <v>887</v>
+      </c>
+      <c r="O613" s="10">
+        <v>3296</v>
+      </c>
+      <c r="P613" s="10">
+        <v>2823</v>
+      </c>
+      <c r="T613" s="10">
+        <v>698</v>
+      </c>
+      <c r="U613" s="61">
+        <v>779</v>
+      </c>
+      <c r="V613" t="s">
+        <v>598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>